<commit_message>
Add Ocean Icon pretty good
</commit_message>
<xml_diff>
--- a/web2/data/records_kriterien.xlsx
+++ b/web2/data/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B14B7D38-DF67-41D1-89F9-D36397B55FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DF1E7E-D401-42BF-8835-24EE65766B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="WR-Youth" sheetId="2" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="58">
   <si>
     <t>50m Retten</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t>Dziacko, Malina</t>
+  </si>
+  <si>
+    <t>Kuhn, Manuel</t>
   </si>
 </sst>
 </file>
@@ -3822,8 +3825,8 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4463,9 +4466,15 @@
         <v>37</v>
       </c>
       <c r="G21"/>
-      <c r="H21" s="35"/>
-      <c r="I21" s="35"/>
-      <c r="J21"/>
+      <c r="H21" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="35" t="s">
+        <v>37</v>
+      </c>
       <c r="L21" s="39"/>
       <c r="M21"/>
       <c r="N21"/>
@@ -4593,8 +4602,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new Fixes und Record smal change
</commit_message>
<xml_diff>
--- a/web2/data/records_kriterien.xlsx
+++ b/web2/data/records_kriterien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DDED9BD-37B3-4A88-A431-88A17C6975A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728C8859-DCA2-4F31-9B1F-7C80859B3F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="WR-Youth" sheetId="2" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="106">
   <si>
     <t>50m Retten</t>
   </si>
@@ -495,6 +495,9 @@
   </si>
   <si>
     <t>CHN</t>
+  </si>
+  <si>
+    <t>Johanna Gnad</t>
   </si>
 </sst>
 </file>
@@ -1980,7 +1983,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -4253,7 +4256,7 @@
   <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5013,8 +5016,8 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5518,7 +5521,7 @@
         <v>37</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="I17" s="8" t="s">
         <v>43</v>
@@ -5527,7 +5530,7 @@
         <v>38</v>
       </c>
       <c r="L17" s="37" t="s">
-        <v>42</v>
+        <v>105</v>
       </c>
       <c r="M17"/>
     </row>

</xml_diff>